<commit_message>
AutoCommit_9 января 2024 г. 11:15:24_SibNout2023
</commit_message>
<xml_diff>
--- a/_2023-2024_2ИСИП-222_Дискретная математика с элементами математической логики_I семестр.xlsx
+++ b/_2023-2024_2ИСИП-222_Дискретная математика с элементами математической логики_I семестр.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -115,6 +115,27 @@
   </si>
   <si>
     <t>Отчислен</t>
+  </si>
+  <si>
+    <t>кол-во</t>
+  </si>
+  <si>
+    <t>аттест.</t>
+  </si>
+  <si>
+    <t>н/а</t>
+  </si>
+  <si>
+    <t>ср балл</t>
+  </si>
+  <si>
+    <t>кач-во,%</t>
+  </si>
+  <si>
+    <t>успев.,%</t>
+  </si>
+  <si>
+    <t>ФИО неуспевающих</t>
   </si>
 </sst>
 </file>
@@ -488,13 +509,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -504,20 +525,92 @@
     <col min="3" max="3" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <f>SUM(D4:D33)</f>
+        <v>27</v>
+      </c>
+      <c r="E3">
+        <f>SUM(F3:I3)</f>
+        <v>27</v>
+      </c>
+      <c r="F3">
+        <f>SUM(F4:F33)</f>
+        <v>24</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:I3" si="0">SUM(G4:G33)</f>
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f>(F2*F3+G2*G3+H2*H3+I2*I3)/E3</f>
+        <v>4.8888888888888893</v>
+      </c>
+      <c r="L3">
+        <f>100*(F3+G3)/D3</f>
+        <v>100</v>
+      </c>
+      <c r="M3">
+        <f>100*(F3+G3+H3)/D3</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -527,8 +620,31 @@
       <c r="C4" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <f>IF(F$2=$C4,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:J19" si="1">IF(G$2=$C4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f>IF(J$2=$C4,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -538,8 +654,31 @@
       <c r="C5" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:J32" si="2">IF(F$2=$C5,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -549,8 +688,31 @@
       <c r="C6" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -560,8 +722,31 @@
       <c r="C7" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -571,8 +756,31 @@
       <c r="C8" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -582,8 +790,31 @@
       <c r="C9" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -593,8 +824,31 @@
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -604,8 +858,31 @@
       <c r="C11" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -615,8 +892,31 @@
       <c r="C12" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -626,8 +926,31 @@
       <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -637,8 +960,31 @@
       <c r="C14" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -648,8 +994,31 @@
       <c r="C15" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -659,8 +1028,31 @@
       <c r="C16" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -670,8 +1062,31 @@
       <c r="C17" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -681,8 +1096,31 @@
       <c r="C18" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -692,8 +1130,31 @@
       <c r="C19" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -703,8 +1164,31 @@
       <c r="C20" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -714,8 +1198,31 @@
       <c r="C21" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -725,8 +1232,31 @@
       <c r="C22" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -736,8 +1266,31 @@
       <c r="C23" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -747,8 +1300,31 @@
       <c r="C24" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -758,8 +1334,31 @@
       <c r="C25" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -769,8 +1368,31 @@
       <c r="C26" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -780,8 +1402,31 @@
       <c r="C27" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -791,8 +1436,31 @@
       <c r="C28" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -802,8 +1470,31 @@
       <c r="C29" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -813,8 +1504,31 @@
       <c r="C30" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -824,8 +1538,31 @@
       <c r="C31" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -834,6 +1571,29 @@
       </c>
       <c r="C32" s="2">
         <v>5</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="33" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>